<commit_message>
working image find in importSealInformation.py
</commit_message>
<xml_diff>
--- a/utilities/seal_information.xlsx
+++ b/utilities/seal_information.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="5400" windowWidth="19200" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organized" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unorganized" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Images" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="271">
   <si>
     <t>Cartridge Mechanical Seals
 Style 18 Seals
@@ -652,6 +653,417 @@
   </si>
   <si>
     <t>All metal surfaces, regardless of how smooth they appear to the naked eye, are not really smooth at all. Observing them under a high powered microscope they project a cross section of saw-toothed irregularities, as illustrated in figure 2. These metal surface asperities complicate the laws of hydrodynamics in that they can poke thru an oil film and cause lubrication failure.,Hydrodynamic lubrication occurs when a very thin film of oil separates two sliding surfaces. This happens when a rotating shaft generates an oil-like wedge equal to the loads on the bearing.,The oil wedge, also referred to as "Hydrodynamic Wedge" is a perfect lubrication and is a lubrication engineer's dream. But because hydrodynamic lubrication requires speeds under moderate loads, it is impossible to maintain these two conditions in every application.,A true hydrodynamic fluid wedge can not be maintained under conditions of high loads and slow speeds. Under these conditions an oil film is either squeezed out, due to pressure, or the sliding motion is inadequate to maintain a lubricating film.</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 18 Single Cartridge High Pressure Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/mStyle18Front.jpg</t>
+  </si>
+  <si>
+    <t>The back of the Fluidol Style 18 Single Cartridge High Pressure Seal</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/mStyle18Rear3.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 18 Single Cartridge High Pressure Seal performance chart.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/18chart.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 19 Double Cartridge Mixer Seal</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/mStyle19.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 19 Double Cartridge Mixer Seal performance chart.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/19chart.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 20 Single Cartridge Mixer Seal</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 20 Single Cartridge Mixer Seal performance chart.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/20chart.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 42 Triple Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_Style 42 Front.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_Style 42-2.jpg</t>
+  </si>
+  <si>
+    <t>A cut away display of the Fluidol Style 42 Triple Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_Style 42 Cut-A-Way 2.jpg</t>
+  </si>
+  <si>
+    <t>The performance and materials chart for the Fluidol Style 42 Double Lip Cartridge Seal</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/42chart.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 44 Double Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_Style 44 Front2.jpg</t>
+  </si>
+  <si>
+    <t>The back of a Fluidol Style 44 Double Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_Style 44 Rear-2.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_Style 44 Rear-3.jpg</t>
+  </si>
+  <si>
+    <t>no images</t>
+  </si>
+  <si>
+    <t>The front of the Fluidol Style 44 Double Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>The back of the Fluidol Style 44 Double Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 01 Component Mechanical Stationary Seat Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style01-Oring.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 01 Component Mechanical Stationary Seat Seal</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style01-04illustration.gif</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 02 Component Mechanical Stationary Seat Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style02Tclamp.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 02 Component Mechanical Stationary Seat Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style02illustration.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 04 Component Mechanical Stationary Seat Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style04cupMount.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 04 Component Mechanical Stationary Seat Seal</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 08 Component Mechanical Stationary Seat Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style08LClamp.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 08 Component Mechanical Stationary Seat Seal.</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 09 Seal for Flygt Pumps.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style09.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 09 Seal for Flygt Pumps.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style09Flygt.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 58 Multi Spring Component Mechanical Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/style58.jpg</t>
+  </si>
+  <si>
+    <t>Chart showing standard sizes of the Fluidol Style 58 Multi Spring Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/chart1.jpg</t>
+  </si>
+  <si>
+    <t>Chart showing the suggested operating limits of the Fluidol Style 58 Multi Spring Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/chart2.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 59 Multi Spring PTFE Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/59.jpg</t>
+  </si>
+  <si>
+    <t>Chart showing standard sizes of the Fluidol Style 59 Multi Spring PTFE Seal.</t>
+  </si>
+  <si>
+    <t>Chart showing the suggested operating limits of the Fluidol Style 59 Multi Spring PTFE Seal.</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 71 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/71.jpg</t>
+  </si>
+  <si>
+    <t>Dimensional data chart of the Fluidol Style 71 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/chart3.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 71 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/71illustrate.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 72 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/72.jpg</t>
+  </si>
+  <si>
+    <t>Dimensional data chart of the Fluidol Style 72 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/72chart.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 72 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/72illustrate.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 73 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/73.jpg</t>
+  </si>
+  <si>
+    <t>Dimensional data chart of the Fluidol Style 73 Elastomer Bellows Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/73chart.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/73illustrate.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 74 Water Pump Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/74.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 74 Water Pump Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/74illustrate.jpg</t>
+  </si>
+  <si>
+    <t>Standard sizing chart of the Fluidol Style 74 Water Pump Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/74chart.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 76 Water Pump Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/76.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 76 Water Pump Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/76illustrate.jpg</t>
+  </si>
+  <si>
+    <t>Standard sizing chart of the Fluidol Style 76 Water Pump Single Spring Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/76chart.jpg</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 80 High Pressure Inside Component Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/80.jpg</t>
+  </si>
+  <si>
+    <t>Performance chart of the Fluidol Style 80 High Pressure Inside Component Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/80chart.jpg</t>
+  </si>
+  <si>
+    <t>Engineer drawing of the Fluidol Style 80 High Pressure Inside Component Seals.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/80illustration.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Enerlon Multiple Element Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/enerlon1.jpg</t>
+  </si>
+  <si>
+    <t>A CAD illustration displaying a cut away of the Fluidol Enerlon Multiple Element Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/enerlon.jpg</t>
+  </si>
+  <si>
+    <t>The front of the Fluidol Style 42 Triple Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Rota-Seal Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/rotaseal.jpg</t>
+  </si>
+  <si>
+    <t>An engineering drawing of the Fluidol Rota-Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/rotasealIllustrate.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Rota-Seal Seal Material Selection chart.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/rotasealTable2.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Rota-Seal Dimensional Information chart.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/rotasealTable1.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 91 General Purpose Seal</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/91.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 91 General Purpose Seal chart of performance and materials.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/91chart.jpg</t>
+  </si>
+  <si>
+    <t>An engineer illustration of the Fluidol Style 91 General Purpose Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/91illustrateStd.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/91illustrateHD.jpg</t>
+  </si>
+  <si>
+    <t>The performance and materials chart for the Fluidol Style 42 Double Lip Cartridge Seal.</t>
+  </si>
+  <si>
+    <t>Picture of the Fluidol Style 10 Multi Spring Component Mechanical Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/10.jpg</t>
+  </si>
+  <si>
+    <t>The performance and materials chart for the Fluidol Style 10 Multi Spring Component Mechanical Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/10chart.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Everseal Multiple Element Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/m_DSC_0073.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/everseal1.jpg</t>
+  </si>
+  <si>
+    <t>A mechanical drawing showing a cut away of the Fluidol Everseal Multiple Element Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/everseal.jpg</t>
+  </si>
+  <si>
+    <t>The performance and materials chart for the Fluidol Everseal Multiple Element Seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/eversealChart.jpg</t>
+  </si>
+  <si>
+    <t>Two of the Fluidol Chek-Tec Style 93 Isolator, one is complete, the other is cut in half.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/93.jpg</t>
+  </si>
+  <si>
+    <t>The Fluidol Style 93 Chek-Tec Seal performance chart.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/93chart.jpg</t>
+  </si>
+  <si>
+    <t>A CAD illustration of the Fluidol Wedgee seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/wedgee.jpg</t>
+  </si>
+  <si>
+    <t>A CAD illustration of the inside of the Fluidol Wedgee seal.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/wedgeeIllustrate.jpg</t>
+  </si>
+  <si>
+    <t>Picture of a series of Magnalube-G products in various size containers.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/magnalube.jpg</t>
+  </si>
+  <si>
+    <t>A chart displaying the illustrated difference between hydrodynamic lubrication and boundary lubrication.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/fig1.jpg</t>
+  </si>
+  <si>
+    <t>An illustration displaying the difficulties with standard high pressure lubricants.</t>
+  </si>
+  <si>
+    <t>https://www.fluidol.com/images/fig4.jpg</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +2306,6 @@
       <c r="A18" t="s">
         <v>104</v>
       </c>
-      <c r="B18" t="s"/>
       <c r="C18" t="s">
         <v>88</v>
       </c>
@@ -2549,14 +2960,1859 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s"/>
+      <c r="C68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76" t="s">
+        <v>40</v>
+      </c>
+      <c r="E76" t="s">
+        <v>41</v>
+      </c>
+      <c r="F76" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" t="s">
+        <v>48</v>
+      </c>
+      <c r="C84" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s"/>
+      <c r="B85" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s"/>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>47</v>
+      </c>
+      <c r="B87" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" t="s">
+        <v>15</v>
+      </c>
+      <c r="E87" t="s">
+        <v>16</v>
+      </c>
+      <c r="F87" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>47</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>47</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>47</v>
+      </c>
+      <c r="B90" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>53</v>
+      </c>
+      <c r="B91" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92" t="s">
+        <v>56</v>
+      </c>
+      <c r="D92" t="s">
+        <v>57</v>
+      </c>
+      <c r="E92" t="s">
+        <v>58</v>
+      </c>
+      <c r="F92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" t="s">
+        <v>16</v>
+      </c>
+      <c r="F93" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s"/>
+      <c r="B94" t="s">
+        <v>60</v>
+      </c>
+      <c r="C94" t="s">
+        <v>61</v>
+      </c>
+      <c r="D94" t="s">
+        <v>62</v>
+      </c>
+      <c r="E94" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" t="s">
+        <v>65</v>
+      </c>
+      <c r="D95" t="s">
+        <v>66</v>
+      </c>
+      <c r="E95" t="s">
+        <v>67</v>
+      </c>
+      <c r="F95" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>45</v>
+      </c>
+      <c r="B96" t="s">
+        <v>69</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>47</v>
+      </c>
+      <c r="B97" t="s">
+        <v>70</v>
+      </c>
+      <c r="C97" t="s">
+        <v>71</v>
+      </c>
+      <c r="D97" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98" t="s">
+        <v>72</v>
+      </c>
+      <c r="C98" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>74</v>
+      </c>
+      <c r="B99" t="s">
+        <v>75</v>
+      </c>
+      <c r="C99" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>77</v>
+      </c>
+      <c r="B100" t="s">
+        <v>78</v>
+      </c>
+      <c r="C100" t="s">
+        <v>79</v>
+      </c>
+      <c r="D100" t="s">
+        <v>80</v>
+      </c>
+      <c r="E100" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>82</v>
+      </c>
+      <c r="B101" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E20" t="s">
+        <v>194</v>
+      </c>
+      <c r="F20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" t="s">
+        <v>205</v>
+      </c>
+      <c r="E22" t="s">
+        <v>200</v>
+      </c>
+      <c r="F22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" t="s">
+        <v>211</v>
+      </c>
+      <c r="F23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>230</v>
+      </c>
+      <c r="B40" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" t="s">
+        <v>232</v>
+      </c>
+      <c r="D40" t="s">
+        <v>233</v>
+      </c>
+      <c r="E40" t="s">
+        <v>234</v>
+      </c>
+      <c r="F40" t="s">
+        <v>235</v>
+      </c>
+      <c r="G40" t="s">
+        <v>236</v>
+      </c>
+      <c r="H40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+      <c r="E41" t="s">
+        <v>242</v>
+      </c>
+      <c r="F41" t="s">
+        <v>243</v>
+      </c>
+      <c r="G41" t="s">
+        <v>242</v>
+      </c>
+      <c r="H41" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" t="s">
+        <v>245</v>
+      </c>
+      <c r="H42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B44" t="s">
+        <v>247</v>
+      </c>
+      <c r="C44" t="s">
+        <v>248</v>
+      </c>
+      <c r="D44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" t="s">
+        <v>251</v>
+      </c>
+      <c r="C46" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" t="s">
+        <v>252</v>
+      </c>
+      <c r="E46" t="s">
+        <v>253</v>
+      </c>
+      <c r="F46" t="s">
+        <v>254</v>
+      </c>
+      <c r="G46" t="s">
+        <v>255</v>
+      </c>
+      <c r="H46" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>257</v>
+      </c>
+      <c r="B47" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" t="s">
+        <v>259</v>
+      </c>
+      <c r="D47" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" t="s">
+        <v>262</v>
+      </c>
+      <c r="C48" t="s">
+        <v>263</v>
+      </c>
+      <c r="D48" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>265</v>
+      </c>
+      <c r="B49" t="s">
+        <v>266</v>
+      </c>
+      <c r="C49" t="s">
+        <v>267</v>
+      </c>
+      <c r="D49" t="s">
+        <v>268</v>
+      </c>
+      <c r="E49" t="s">
+        <v>269</v>
+      </c>
+      <c r="F49" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>230</v>
+      </c>
+      <c r="B50" t="s">
+        <v>231</v>
+      </c>
+      <c r="C50" t="s">
+        <v>232</v>
+      </c>
+      <c r="D50" t="s">
+        <v>233</v>
+      </c>
+      <c r="E50" t="s">
+        <v>234</v>
+      </c>
+      <c r="F50" t="s">
+        <v>235</v>
+      </c>
+      <c r="G50" t="s">
+        <v>236</v>
+      </c>
+      <c r="H50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>